<commit_message>
plots for normal prior
</commit_message>
<xml_diff>
--- a/references/Log.xlsx
+++ b/references/Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14840" windowHeight="16840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>simulate data with mn for random intercept and t3 for random error, called mn_t2_100.Rdata</t>
   </si>
@@ -36,18 +36,12 @@
     <t>the bias is ok but the density plot didn't work</t>
   </si>
   <si>
-    <t>simulate data withN(1, 4) for random intercept, MN for random slope and t3 for random error, called mn_t2_2re_30.Rdata</t>
-  </si>
-  <si>
     <t>adjust the model file v2 to a new version v3 to incoperate the random slope</t>
   </si>
   <si>
     <t>us DPM to model both random effects</t>
   </si>
   <si>
-    <t>simulate data withN(0, 4) for random intercept, MN for random slope and t3 for random error, called mn_t2_2re_30_new.Rdata</t>
-  </si>
-  <si>
     <t>x is also changed to have mean 0</t>
   </si>
   <si>
@@ -61,13 +55,108 @@
   </si>
   <si>
     <t>use model_v3 to fit the data</t>
+  </si>
+  <si>
+    <t>simulate data with N(1, 4) for random intercept, MN for random slope and t3 for random error, called mn_t2_2re_30.Rdata</t>
+  </si>
+  <si>
+    <t>two posterior data named are mn_t3_2re_10.Rdata and mn_t3_2re_new_10.Rdata</t>
+  </si>
+  <si>
+    <t>simulate data with N(0, 4) for random intercept, MN for random slope and t3 for random error, called mn_t2_2re_30_new.Rdata</t>
+  </si>
+  <si>
+    <t>use only the first 10 data sets</t>
+  </si>
+  <si>
+    <t>Get results from previous simulation studies (using v3 for two data sets simulated above )and plot the densities to check the fit of the predictions</t>
+  </si>
+  <si>
+    <t>create normal model file</t>
+  </si>
+  <si>
+    <r>
+      <t>Run simulation on the complete 30 data sets using</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CDPM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prior for BLQMM</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run simulation on the complete 30 data sets using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>normal prior</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for BLQMM</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">run </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>additional 20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and combine with the previous results, run only on new data</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,6 +216,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -170,10 +266,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -212,18 +314,24 @@
     <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -557,24 +665,24 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="66.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -590,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -621,16 +729,16 @@
     <row r="8" spans="1:3" ht="30">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
       <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -639,76 +747,101 @@
     <row r="11" spans="1:3" ht="30">
       <c r="A11" s="10"/>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="10"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="10"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="A14" s="9">
+        <v>41884</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" ht="45">
       <c r="A15" s="10"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45">
       <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="10"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:3">
       <c r="A19" s="10"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:3">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:3">
       <c r="A21" s="10"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:3">
       <c r="A22" s="10"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:3">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:3">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:3">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:3">
       <c r="A26" s="10"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:3">
       <c r="A27" s="10"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:3">
       <c r="A28" s="10"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:3">
       <c r="A29" s="10"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:3">
       <c r="A30" s="10"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:3">
       <c r="A31" s="10"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:3">
       <c r="A32" s="10"/>
     </row>
   </sheetData>

</xml_diff>